<commit_message>
added urls and timestamps
</commit_message>
<xml_diff>
--- a/events2.xlsx
+++ b/events2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/squiresrb/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAEEFBE-39EE-B046-93BA-0F1A7B5E16AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9047F9-DE32-4846-BC5C-074E5E9F678E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3520" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>type</t>
   </si>
@@ -106,21 +106,6 @@
     <t>Overview of real-world data and statistical analysis concepts, data analysis and visualization of a real-world dataset</t>
   </si>
   <si>
-    <t>Statistics</t>
-  </si>
-  <si>
-    <t>Statistical hypothesis testing in Prism</t>
-  </si>
-  <si>
-    <t>Overview: This workshop will focus on how to choose an appropriate statistical test given data and hypothesis. It will include a hands on section for attendees to practice how to run these tests using Prism. Specific topic include the following: unpaired t-test, paired t-test, ordinary one-way ANOVA, repeated measures one-way ANOVA and non-parametric tests, Chi-square test and Fisher’s exact test.</t>
-  </si>
-  <si>
-    <t>1:00PM</t>
-  </si>
-  <si>
-    <t>12:00PM</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -130,16 +115,13 @@
     <t>Remote</t>
   </si>
   <si>
-    <t>Bethesda, MD</t>
-  </si>
-  <si>
     <t>RSNA 2023 Test</t>
   </si>
   <si>
     <t>R</t>
   </si>
   <si>
-    <t>Prism</t>
+    <t>https://nih.zoomgov.com/j/1618272266?pwd=U281WDVxLzcyN0VNdkd3d3kzQ2d3Zz09</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,7 +1048,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1">
         <v>45256</v>
@@ -1109,23 +1091,26 @@
       <c r="D3" s="1">
         <v>45481</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
+      <c r="E3">
+        <v>1720443600</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>21</v>
@@ -1144,23 +1129,26 @@
       <c r="D4" s="1">
         <v>45488</v>
       </c>
-      <c r="E4" t="s">
-        <v>31</v>
+      <c r="E4">
+        <v>1721048400</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
       <c r="K4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>21</v>
@@ -1179,23 +1167,26 @@
       <c r="D5" s="1">
         <v>45495</v>
       </c>
-      <c r="E5" t="s">
-        <v>31</v>
+      <c r="E5">
+        <v>1721653200</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
         <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>21</v>
@@ -1214,66 +1205,34 @@
       <c r="D6" s="1">
         <v>45502</v>
       </c>
-      <c r="E6" t="s">
-        <v>31</v>
+      <c r="E6">
+        <v>1722258000</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J6" t="s">
         <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="1">
-        <v>45413</v>
-      </c>
-      <c r="D7" s="1">
-        <v>45413</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update dates of training and tried to add timestamp calc
</commit_message>
<xml_diff>
--- a/events2.xlsx
+++ b/events2.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/booirizarryy/Documents/nbp_events_niaid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/squiresrb/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B274C6-9919-DE40-A424-00021FC9FB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED8472B-3826-F54F-B584-BF7F03397BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="2180" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>type</t>
   </si>
@@ -139,10 +152,22 @@
     <t>Darrel Hurt</t>
   </si>
   <si>
-    <t>Richard Squires</t>
-  </si>
-  <si>
     <t>David Liou</t>
+  </si>
+  <si>
+    <t>Mina Peyton / Yuyan Yi</t>
+  </si>
+  <si>
+    <t>date_to_timestamp</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>time_fraction</t>
+  </si>
+  <si>
+    <t>timestamp_calc</t>
   </si>
 </sst>
 </file>
@@ -632,10 +657,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1011,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1023,17 +1050,22 @@
     <col min="2" max="2" width="34.83203125" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="72.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="255.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="119.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.33203125" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1047,34 +1079,46 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1087,32 +1131,47 @@
       <c r="D2" s="1">
         <v>45259</v>
       </c>
-      <c r="E2">
-        <v>1700956851</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1700956800.5416667</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>38</v>
       </c>
+      <c r="P2" s="2">
+        <f>(C2-DATE(1970,1,1))*86400</f>
+        <v>1700956800</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>13/24</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="R2" s="2">
+        <f>P2+Q2</f>
+        <v>1700956800.5416667</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1120,40 +1179,55 @@
         <v>20</v>
       </c>
       <c r="C3" s="1">
-        <v>45481</v>
+        <v>45534</v>
       </c>
       <c r="D3" s="1">
-        <v>45481</v>
-      </c>
-      <c r="E3">
-        <v>1720443600</v>
-      </c>
-      <c r="F3" t="s">
+        <v>45534</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1724976000.5416667</v>
+      </c>
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>29</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M3" t="s">
-        <v>39</v>
+      <c r="N3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="2">
+        <f>(C3-DATE(1970,1,1))*86400</f>
+        <v>1724976000</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>13/24</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="R3" s="2">
+        <f>P3+Q3</f>
+        <v>1724976000.5416667</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1161,40 +1235,55 @@
         <v>23</v>
       </c>
       <c r="C4" s="1">
-        <v>45488</v>
+        <v>45541</v>
       </c>
       <c r="D4" s="1">
-        <v>45488</v>
-      </c>
-      <c r="E4">
-        <v>1721048400</v>
-      </c>
-      <c r="F4" t="s">
+        <v>45541</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1725580800.5416667</v>
+      </c>
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>29</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M4" t="s">
-        <v>39</v>
+      <c r="N4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="2">
+        <f>(C4-DATE(1970,1,1))*86400</f>
+        <v>1725580800</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>13/24</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="R4" s="2">
+        <f>P4+Q4</f>
+        <v>1725580800.5416667</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1202,40 +1291,55 @@
         <v>24</v>
       </c>
       <c r="C5" s="1">
-        <v>45495</v>
+        <v>45548</v>
       </c>
       <c r="D5" s="1">
-        <v>45495</v>
-      </c>
-      <c r="E5">
-        <v>1721653200</v>
-      </c>
-      <c r="F5" t="s">
+        <v>45548</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1726185600.5416667</v>
+      </c>
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>22</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M5" t="s">
-        <v>39</v>
+      <c r="N5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="2">
+        <f>(C5-DATE(1970,1,1))*86400</f>
+        <v>1726185600</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>13/24</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="R5" s="2">
+        <f>P5+Q5</f>
+        <v>1726185600.5416667</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1243,40 +1347,55 @@
         <v>26</v>
       </c>
       <c r="C6" s="1">
-        <v>45502</v>
+        <v>45555</v>
       </c>
       <c r="D6" s="1">
-        <v>45502</v>
-      </c>
-      <c r="E6">
-        <v>1722258000</v>
-      </c>
-      <c r="F6" t="s">
+        <v>45555</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1726790400.5416667</v>
+      </c>
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>33</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>29</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>28</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>27</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M6" t="s">
-        <v>39</v>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="2">
+        <f>(C6-DATE(1970,1,1))*86400</f>
+        <v>1726790400</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>13/24</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="R6" s="2">
+        <f>P6+Q6</f>
+        <v>1726790400.5416667</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1289,26 +1408,41 @@
       <c r="D7" s="1">
         <v>45523</v>
       </c>
-      <c r="E7" s="2">
-        <v>1724089786</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1724025600.5416667</v>
+      </c>
+      <c r="G7" t="s">
         <v>30</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>29</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>28</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>36</v>
       </c>
-      <c r="M7" t="s">
-        <v>40</v>
+      <c r="N7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="2">
+        <f>(C7-DATE(1970,1,1))*86400</f>
+        <v>1724025600</v>
+      </c>
+      <c r="Q7" s="2">
+        <f>13/24</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="R7" s="2">
+        <f>P7+Q7</f>
+        <v>1724025600.5416667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated events with fall 2024 trainings
</commit_message>
<xml_diff>
--- a/events2.xlsx
+++ b/events2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/squiresrb/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5520825F-34F0-8A4D-893D-06C7F02AB297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6987DEE-345F-E347-8044-7261DEC80211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5000" yWindow="-20360" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events2" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>type</t>
   </si>
@@ -138,6 +138,69 @@
   </si>
   <si>
     <t>https://nih.zoomgov.com/meeting/register/vJItdO6qqT8vHcm1uNVl7qLADShJAAiY20M</t>
+  </si>
+  <si>
+    <t>16S Amplicon Sequence Analysis with DADA2 and R</t>
+  </si>
+  <si>
+    <t>Next Generation Sequencing</t>
+  </si>
+  <si>
+    <t>16S, R</t>
+  </si>
+  <si>
+    <t>Shotgun Metagenomics Using Nephele</t>
+  </si>
+  <si>
+    <t>Spatial Transcriptomics Introduction and Tutorial (Part 2)</t>
+  </si>
+  <si>
+    <t>Spatial Transcriptomics Introduction and Tutorial (Part I)</t>
+  </si>
+  <si>
+    <t>Statistical Analysis of Microbiome Data</t>
+  </si>
+  <si>
+    <t>Microbiome</t>
+  </si>
+  <si>
+    <t>Learn the nuts and bolts of 16S amplicon microbiome sequence analysis with DADA2. This hands-on tutorial will walk through all key steps in detail, providing understanding about each component and common pitfalls. Feel free to bring data from a current project, too! While most of the training will be taught in R, limited R coding experience will be necessary.</t>
+  </si>
+  <si>
+    <t>Learn microbiome analysis basics in R with phyloseq. This workshop will cover different types of analysis frequently used in microbiome studies, including sample diversity, community composition, and differential taxa. The techniques we learn will be applicable to both amplicon and metagenomic data.</t>
+  </si>
+  <si>
+    <t>Introduction to spatial transcriptomics methods and concepts for STx data analysis.</t>
+  </si>
+  <si>
+    <t>Hands-on workshop using R and Seurat to analyze an example spatial transcriptomics dataset.</t>
+  </si>
+  <si>
+    <t>A hands-on workshop for analyzing metagenomes in the open-source microbiome application Nephele. Participants will first learn how to navigate Nephele and process their reads to trim and filter for quality. They will then learn how to run their data through the WGSA2 pipeline to assemble metagenomic reads, obtain taxonomic and functional annotations and abundances for downstream analyses, generate metagenome assembled genomes, explore viruses, and more.</t>
+  </si>
+  <si>
+    <t>https://nih.zoomgov.com/meeting/register/vJIsfuGrqDgoEq06dtCsG9iZvpV3u3bbOuE</t>
+  </si>
+  <si>
+    <t>https://nih.zoomgov.com/meeting/register/vJItd-usqTkoHGnlbkmiHP_oL82zIH1jFxk</t>
+  </si>
+  <si>
+    <t>https://nih.zoomgov.com/meeting/register/vJItceyupjMuH9fwvmt_zqUXFIM4p6BwCgo</t>
+  </si>
+  <si>
+    <t>https://nih.zoomgov.com/meeting/register/vJItd-isrjojGpCH_Sr9xzWmdhI8YTR2g4k</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://nih.zoomgov.com/meeting/register/vJItc--urTkiHBI4Gh5kRuqucJCkFhb-w-4</t>
+  </si>
+  <si>
+    <t>microbiome</t>
+  </si>
+  <si>
+    <t>transcriptomics</t>
+  </si>
+  <si>
+    <t>BCBB SME</t>
   </si>
 </sst>
 </file>
@@ -630,12 +693,13 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1012,16 +1076,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" customWidth="1"/>
@@ -1136,15 +1200,15 @@
         <v>26</v>
       </c>
       <c r="P2" s="2">
-        <f t="shared" ref="P2:P5" si="0">(C2-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="P2:P10" si="0">(C2-DATE(1970,1,1))*86400</f>
         <v>1724976000</v>
       </c>
       <c r="Q2" s="2">
-        <f t="shared" ref="Q2:Q5" si="1">13/24</f>
+        <f t="shared" ref="Q2:Q10" si="1">13/24</f>
         <v>0.54166666666666663</v>
       </c>
       <c r="R2" s="2">
-        <f t="shared" ref="R2:R5" si="2">P2+Q2</f>
+        <f t="shared" ref="R2:R10" si="2">P2+Q2</f>
         <v>1724976000.5416667</v>
       </c>
     </row>
@@ -1316,7 +1380,293 @@
         <v>1726790400.5416667</v>
       </c>
     </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45588</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45588</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1729641600.5833333</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>55</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="0"/>
+        <v>1729641600</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>14/24</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="R6" s="2">
+        <f t="shared" si="2"/>
+        <v>1729641600.5833333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45597</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45597</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1730419200.5833333</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="0"/>
+        <v>1730419200</v>
+      </c>
+      <c r="Q7" s="2">
+        <f>14/24</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" si="2"/>
+        <v>1730419200.5833333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45604</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45604</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1731024000.5833333</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" t="s">
+        <v>55</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="0"/>
+        <v>1731024000</v>
+      </c>
+      <c r="Q8" s="2">
+        <f>14/24</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="2"/>
+        <v>1731024000.5833333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45600</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45600</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1730678400.5416667</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="0"/>
+        <v>1730678400</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="2"/>
+        <v>1730678400.5416667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45611</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45611</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1731628800.5416667</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" t="s">
+        <v>55</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="0"/>
+        <v>1731628800</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="2"/>
+        <v>1731628800.5416667</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{0265776D-23F7-4441-AD9E-6BFE457E38B2}"/>
+    <hyperlink ref="H7" r:id="rId2" xr:uid="{DC25BF45-3904-C04B-B53C-EF2D382E6BB8}"/>
+    <hyperlink ref="H8" r:id="rId3" xr:uid="{65F23710-E528-434A-911E-763CDAA02F1D}"/>
+    <hyperlink ref="H9" r:id="rId4" xr:uid="{897BF1F6-E133-2244-8454-DDB795FA808D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>